<commit_message>
added a additional constrains and more detailed README
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agaspariunas.LIFEARC\projects\studies_endpoint_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FF506B-C802-465A-981B-0A4D75CE60E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC34622B-2472-4E3B-B9CB-EEF1F029BC0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{350406E5-7FBB-4BED-BF13-A26B7717BB03}"/>
+    <workbookView xWindow="5925" yWindow="-13740" windowWidth="19185" windowHeight="10095" xr2:uid="{350406E5-7FBB-4BED-BF13-A26B7717BB03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>sample_id</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>time_step</t>
+  </si>
+  <si>
+    <t>eln_id</t>
   </si>
 </sst>
 </file>
@@ -468,35 +471,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65F6FC5-B2FD-4E96-BEEB-B2910050B411}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="36.90625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="17" style="3" customWidth="1"/>
-    <col min="9" max="9" width="40.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" style="3" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="22.54296875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="17" style="3" customWidth="1"/>
-    <col min="18" max="18" width="32.90625" style="5" customWidth="1"/>
-    <col min="19" max="19" width="10.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="19.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.1796875" style="3"/>
+    <col min="2" max="3" width="12.6328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="36.90625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="17" style="3" customWidth="1"/>
+    <col min="10" max="10" width="40.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" style="3" customWidth="1"/>
+    <col min="13" max="13" width="15.453125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="22.54296875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="15.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="17" style="3" customWidth="1"/>
+    <col min="19" max="19" width="32.90625" style="5" customWidth="1"/>
+    <col min="20" max="20" width="10.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="19.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,64 +507,67 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -572,15 +578,16 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="1"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="1"/>
+      <c r="O4" s="4"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -590,13 +597,14 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="J5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>